<commit_message>
Se agrega campo fecha vencimiento en cargues masivos, se agrega campo para guardar request que se envia a factus, campo para guardar respuesta de api factus en caso de error esto para factura electronica y nota credito electronica
</commit_message>
<xml_diff>
--- a/archivos/Cargue masivo/Editar producto masivo/EditarProductoMasivo.xlsx
+++ b/archivos/Cargue masivo/Editar producto masivo/EditarProductoMasivo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kadye\Documents\RUBEN\SBX\SBX Local V2\sbx\archivos\Cargue masivo\Editar producto masivo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B840C923-FBA5-4753-B9A8-DA3AE79B4A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C93B1D4-C8F9-474D-BD5A-2618059ACD8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-75" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Sku</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Cantidad</t>
+  </si>
+  <si>
+    <t>FechaVencimiento</t>
   </si>
 </sst>
 </file>
@@ -463,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2875"/>
+  <dimension ref="A1:K2875"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -479,9 +482,10 @@
     <col min="8" max="8" width="19.44140625" style="11" customWidth="1"/>
     <col min="9" max="9" width="13.109375" style="11" customWidth="1"/>
     <col min="10" max="10" width="11.5546875" style="11"/>
+    <col min="11" max="11" width="19.5546875" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>7</v>
       </c>
@@ -512,51 +516,54 @@
       <c r="J1" s="13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D2" s="1"/>
       <c r="H2" s="15"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.3">

</xml_diff>